<commit_message>
resolving merge conflicts; restoring from stash
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-AccountExtension.xlsx
+++ b/output/StructureDefinition-AccountExtension.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>0.2.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-03-17T13:26:51-04:00</t>
+    <t>2022-04-07T11:11:08-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>